<commit_message>
Test cases for TDD sprint #2
</commit_message>
<xml_diff>
--- a/test/Test_cases_for_TDD_sprint__2.xlsx
+++ b/test/Test_cases_for_TDD_sprint__2.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="36">
   <si>
     <t>Test cases</t>
   </si>
@@ -112,13 +112,13 @@
     <t>xxx xxx A</t>
   </si>
   <si>
+    <t>xxx xxx xxx xxx C</t>
+  </si>
+  <si>
     <t>xxx A.</t>
   </si>
   <si>
     <t>xxx xxx. C</t>
-  </si>
-  <si>
-    <t>xxx xxx xxx xxx C</t>
   </si>
 </sst>
 </file>
@@ -201,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -255,9 +255,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
@@ -481,6 +478,8 @@
     <col customWidth="1" min="1" max="1" width="14.43"/>
     <col customWidth="1" min="2" max="2" width="19.0"/>
     <col customWidth="1" min="3" max="3" width="11.86"/>
+    <col customWidth="1" min="4" max="4" width="36.57"/>
+    <col customWidth="1" min="6" max="6" width="23.0"/>
     <col customWidth="1" min="9" max="9" width="22.57"/>
     <col customWidth="1" min="10" max="10" width="63.43"/>
   </cols>
@@ -1296,7 +1295,7 @@
     </row>
     <row r="33">
       <c r="A33" s="10">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>32</v>
@@ -1304,11 +1303,15 @@
       <c r="C33" s="10">
         <v>1.0</v>
       </c>
-      <c r="D33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>33</v>
+      </c>
       <c r="E33" s="17">
         <v>1.0</v>
       </c>
-      <c r="F33" s="10"/>
+      <c r="F33" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="G33" s="17">
         <v>1.0</v>
       </c>
@@ -1317,16 +1320,20 @@
     <row r="34">
       <c r="A34" s="11"/>
       <c r="B34" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C34" s="10">
         <v>1.0</v>
       </c>
-      <c r="D34" s="10"/>
+      <c r="D34" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="E34" s="17">
         <v>1.0</v>
       </c>
-      <c r="F34" s="10"/>
+      <c r="F34" s="10" t="s">
+        <v>34</v>
+      </c>
       <c r="G34" s="17">
         <v>1.0</v>
       </c>
@@ -1335,16 +1342,20 @@
     <row r="35">
       <c r="A35" s="11"/>
       <c r="B35" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="D35" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="D35" s="10"/>
       <c r="E35" s="17">
         <v>1.0</v>
       </c>
-      <c r="F35" s="10"/>
+      <c r="F35" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="G35" s="17">
         <v>1.0</v>
       </c>
@@ -1353,17 +1364,21 @@
     <row r="36">
       <c r="A36" s="11"/>
       <c r="B36" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C36" s="10">
         <v>1.0</v>
       </c>
-      <c r="D36" s="18"/>
-      <c r="E36" s="19">
-        <v>1.0</v>
-      </c>
-      <c r="F36" s="18"/>
-      <c r="G36" s="19">
+      <c r="D36" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E36" s="18">
+        <v>1.0</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G36" s="18">
         <v>1.0</v>
       </c>
       <c r="I36" s="16"/>

</xml_diff>